<commit_message>
alterações no script do banco de dados, alteração na documentação, criação da tela de sessões de meditação, estilização da sidebar
</commit_message>
<xml_diff>
--- a/Tecnologia da informação/LotusTech_Product Backlog.xlsx
+++ b/Tecnologia da informação/LotusTech_Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Documentos\LotusTech\Tecnologia da informação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499FD742-310D-4959-9546-51B53474FC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30589EE0-EE3C-49E7-BCD1-8E7EDCAE4770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D2139C2F-4166-47FE-8236-B6B2F48D4D38}"/>
   </bookViews>
@@ -130,21 +130,7 @@
 (Back-end)</t>
   </si>
   <si>
-    <t xml:space="preserve">O banco de dados terá as tabelas de usuário, registro de atividade e registro de bem-estar </t>
-  </si>
-  <si>
-    <t>Tela Informativa
-(Front-end)</t>
-  </si>
-  <si>
-    <t>Tela Informativa
-(Back-end)</t>
-  </si>
-  <si>
     <t>Essa tela será uma das opções da sidebar para navegação mais otimizada da solução</t>
-  </si>
-  <si>
-    <t>Tela onde haverá informações sobre os benefícios da meditação, tecnicas de atenção plena e saúde mental e artigos relacionados a saúde mental</t>
   </si>
   <si>
     <t>Tela Perfil
@@ -317,6 +303,20 @@
   </si>
   <si>
     <t>Requisito</t>
+  </si>
+  <si>
+    <t>O banco de dados terá as tabelas de usuário, endereço, rastreamento, gamificação e infoMeditação</t>
+  </si>
+  <si>
+    <t>Tela onde haverá sessões de meditação guiada e benefícios da sessão</t>
+  </si>
+  <si>
+    <t>Tela Sessões
+(Front-end)</t>
+  </si>
+  <si>
+    <t>Tela Sessões
+(Back-end)</t>
   </si>
 </sst>
 </file>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCD47BA-8203-40AE-8F41-4F8BC3EF1468}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +804,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7" t="s">
@@ -862,13 +862,13 @@
         <v>5</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="S2" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -901,10 +901,10 @@
         <v>8</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="S3" s="3">
         <f>SUM(N2:N22)</f>
@@ -920,7 +920,7 @@
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -941,10 +941,10 @@
         <v>5</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="S4" s="3">
         <f>SUM(N19:N21,N9)</f>
@@ -981,10 +981,10 @@
         <v>8</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="S5" s="3">
         <f>SUM(N2:N7)</f>
@@ -993,7 +993,7 @@
     </row>
     <row r="6" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>26</v>
@@ -1021,10 +1021,10 @@
         <v>5</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S6" s="3">
         <f>SUM(N10:N15)</f>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="7" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>27</v>
@@ -1061,10 +1061,10 @@
         <v>5</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S7" s="3">
         <f>SUM(N16:N18,N8,N22)</f>
@@ -1073,14 +1073,14 @@
     </row>
     <row r="8" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1095,25 +1095,25 @@
         <v>1</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="N8" s="3">
         <v>13</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1134,19 +1134,19 @@
         <v>5</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -1167,19 +1167,19 @@
         <v>5</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1200,19 +1200,19 @@
         <v>8</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -1227,25 +1227,25 @@
         <v>1</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N12" s="3">
         <v>3</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1266,19 +1266,19 @@
         <v>8</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1287,7 +1287,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>1</v>
@@ -1299,19 +1299,19 @@
         <v>5</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1320,7 +1320,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>1</v>
@@ -1332,19 +1332,19 @@
         <v>8</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -1353,31 +1353,31 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N16" s="3">
         <v>3</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1389,28 +1389,28 @@
         <v>6</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N17" s="3">
         <v>3</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1422,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>4</v>
@@ -1431,19 +1431,19 @@
         <v>5</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1455,28 +1455,28 @@
         <v>6</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N19" s="3">
         <v>3</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1488,28 +1488,28 @@
         <v>6</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N20" s="3">
         <v>3</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -1521,28 +1521,28 @@
         <v>0</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="N21" s="3">
         <v>21</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -1554,7 +1554,7 @@
         <v>6</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>2</v>
@@ -1563,21 +1563,29 @@
         <v>8</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:J16"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="B12:C12"/>
@@ -1594,24 +1602,16 @@
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:J5"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:J22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:J9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
substituindo o perfil pela tela sobre
</commit_message>
<xml_diff>
--- a/Tecnologia da informação/LotusTech_Product Backlog.xlsx
+++ b/Tecnologia da informação/LotusTech_Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Documentos\LotusTech\Tecnologia da informação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30589EE0-EE3C-49E7-BCD1-8E7EDCAE4770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C721FD2-4BB5-47E1-B904-5EF18CFD3987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D2139C2F-4166-47FE-8236-B6B2F48D4D38}"/>
   </bookViews>
@@ -133,18 +133,10 @@
     <t>Essa tela será uma das opções da sidebar para navegação mais otimizada da solução</t>
   </si>
   <si>
-    <t>Tela Perfil
-(Front-end)</t>
-  </si>
-  <si>
     <t>O software deverá permitir a opção de cadastro do usuário, para isso o usuário deverá informar o nome, um e-mail válido e uma senha, confirmando no campo abaixo. Deverá conter também um botão de redirecionamento para a tela de Login</t>
   </si>
   <si>
     <t>Desejável</t>
-  </si>
-  <si>
-    <t>Tela Perfil
-(Back-end)</t>
   </si>
   <si>
     <t>G</t>
@@ -281,12 +273,6 @@
     <t>Apresentação dos slides</t>
   </si>
   <si>
-    <t xml:space="preserve"> O perfil deverá conter as informações pessoais como celular, email, foto, nome, botão para editar essas informações e uma amostra grafica do seu nivel conforme seu envolvimento com a plataforma</t>
-  </si>
-  <si>
-    <t>Sendo uma das opções da sidebar, nessa tela as informações serão retiradas do banco de dados</t>
-  </si>
-  <si>
     <t>Cada etapa concluída do projeto deverá que ser comunicada na ferramenta de gestão (Trello)</t>
   </si>
   <si>
@@ -297,9 +283,6 @@
   </si>
   <si>
     <t>Com base nos dados do banco de dados que foram fornecidos pelos usuários, os dados serão convertidos em metricas para fazer uma amostra grafica aos usuários</t>
-  </si>
-  <si>
-    <t>O software oferecerá uma tela onde os usuários poderão adicionar registrar sua emoção, nivel de estresse e progresso na pratica da meditação onde haverá graficos com seu progresso ao longo do tempo</t>
   </si>
   <si>
     <t>Requisito</t>
@@ -317,6 +300,23 @@
   <si>
     <t>Tela Sessões
 (Back-end)</t>
+  </si>
+  <si>
+    <t>Tela sobre
+(Back-end)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tela onde haverá o motivo pelo qual estou fazendo o site </t>
+  </si>
+  <si>
+    <t>Tela Sobre
+(Front-end)</t>
+  </si>
+  <si>
+    <t>Uma das opções da sidebar</t>
+  </si>
+  <si>
+    <t>O software oferecerá uma tela onde os usuários poderão adicionar registrar sua emoção e nivel de estresse onde haverá graficos com seu progresso ao longo do tempo</t>
   </si>
 </sst>
 </file>
@@ -434,23 +434,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>421993</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>12058</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>523876</xdr:colOff>
+      <xdr:colOff>289367</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>115868</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2">
+        <xdr:cNvPr id="4" name="Imagem 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36C4767B-AAFF-3F13-3999-4A21876F2EB6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B8A6404-F1C5-7728-3690-27346FF03F58}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -466,13 +466,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="25123" r="21078"/>
+        <a:srcRect l="23889" r="22437"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12372975" y="190500"/>
-          <a:ext cx="4181476" cy="4371974"/>
+          <a:off x="12237816" y="204969"/>
+          <a:ext cx="4171709" cy="4371975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCD47BA-8203-40AE-8F41-4F8BC3EF1468}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +804,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7" t="s">
@@ -862,13 +862,13 @@
         <v>5</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -901,14 +901,14 @@
         <v>8</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="S3" s="3">
         <f>SUM(N2:N22)</f>
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -920,7 +920,7 @@
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -941,10 +941,10 @@
         <v>5</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="S4" s="3">
         <f>SUM(N19:N21,N9)</f>
@@ -981,10 +981,10 @@
         <v>8</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="S5" s="3">
         <f>SUM(N2:N7)</f>
@@ -993,7 +993,7 @@
     </row>
     <row r="6" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>26</v>
@@ -1021,19 +1021,19 @@
         <v>5</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S6" s="3">
         <f>SUM(N10:N15)</f>
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>27</v>
@@ -1061,10 +1061,10 @@
         <v>5</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S7" s="3">
         <f>SUM(N16:N18,N8,N22)</f>
@@ -1073,14 +1073,14 @@
     </row>
     <row r="8" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1095,25 +1095,25 @@
         <v>1</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N8" s="3">
         <v>13</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1134,19 +1134,19 @@
         <v>5</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -1167,15 +1167,15 @@
         <v>5</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
@@ -1200,19 +1200,19 @@
         <v>8</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -1221,31 +1221,31 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N12" s="3">
         <v>3</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1254,31 +1254,31 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="N13" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1287,7 +1287,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>1</v>
@@ -1299,19 +1299,19 @@
         <v>5</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1320,7 +1320,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>1</v>
@@ -1332,19 +1332,19 @@
         <v>8</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -1353,31 +1353,31 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N16" s="3">
         <v>3</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1389,28 +1389,28 @@
         <v>6</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N17" s="3">
         <v>3</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1422,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>4</v>
@@ -1431,19 +1431,19 @@
         <v>5</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1455,28 +1455,28 @@
         <v>6</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N19" s="3">
         <v>3</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1488,28 +1488,28 @@
         <v>6</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N20" s="3">
         <v>3</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -1521,28 +1521,28 @@
         <v>0</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N21" s="3">
         <v>21</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -1554,7 +1554,7 @@
         <v>6</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>2</v>
@@ -1563,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>